<commit_message>
more rececent update to files
</commit_message>
<xml_diff>
--- a/manual_reference_data_tables_for_IGDB_API.xlsx
+++ b/manual_reference_data_tables_for_IGDB_API.xlsx
@@ -24,7 +24,6 @@
     <sheet state="visible" name="release_date_region" sheetId="19" r:id="rId22"/>
     <sheet state="visible" name="platform_website_enums_category" sheetId="20" r:id="rId23"/>
     <sheet state="visible" name="website_enums_category" sheetId="21" r:id="rId24"/>
-    <sheet state="visible" name="Sheet11" sheetId="22" r:id="rId25"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -577,10 +576,6 @@
 </file>
 
 <file path=xl/drawings/drawing21.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing22.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -2478,20 +2473,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
-  <sheetData/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>

</xml_diff>